<commit_message>
Added a heading to the In Box column
</commit_message>
<xml_diff>
--- a/Hardware/Electronics/Data Acquisition Board/DAQ Board/BoM.xlsx
+++ b/Hardware/Electronics/Data Acquisition Board/DAQ Board/BoM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Willie\Documents\Uni\Newcastle\4 Fourth Year\1 Final Year Project\trunk\Hardware\Electronics\Data Acquisition Board\DAQ Board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{708AAB3A-10F2-412E-8838-F3A31998DD5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6264869-D11C-4F6E-AD7B-9B73AB988FDB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{6508AD80-5785-495C-937B-5500FE895B69}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1671" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1671" uniqueCount="353">
   <si>
     <t xml:space="preserve">    ADC1</t>
   </si>
@@ -1094,6 +1094,9 @@
   </si>
   <si>
     <t>In Box</t>
+  </si>
+  <si>
+    <t>ADS1299 Analog Front End</t>
   </si>
 </sst>
 </file>
@@ -1178,24 +1181,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF70AD47"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF70AD47"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -5729,8 +5715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE20D855-7A6D-49D9-8684-28A19F146B00}">
   <dimension ref="B1:K144"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+    <sheetView tabSelected="1" topLeftCell="A112" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G149" sqref="G149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5974,7 +5960,7 @@
         <v>1</v>
       </c>
       <c r="G8">
-        <f>1-F8</f>
+        <f t="shared" ref="G8:G39" si="0">1-F8</f>
         <v>0</v>
       </c>
       <c r="H8" s="4" t="s">
@@ -6005,7 +5991,7 @@
         <v>1</v>
       </c>
       <c r="G9">
-        <f>1-F9</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H9" s="4" t="s">
@@ -6036,7 +6022,7 @@
         <v>1</v>
       </c>
       <c r="G10">
-        <f>1-F10</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H10" s="4" t="s">
@@ -6067,7 +6053,7 @@
         <v>1</v>
       </c>
       <c r="G11">
-        <f>1-F11</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H11" s="4" t="s">
@@ -6098,7 +6084,7 @@
         <v>1</v>
       </c>
       <c r="G12">
-        <f>1-F12</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H12" s="4" t="s">
@@ -6129,7 +6115,7 @@
         <v>1</v>
       </c>
       <c r="G13">
-        <f>1-F13</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H13" s="4" t="s">
@@ -6160,7 +6146,7 @@
         <v>1</v>
       </c>
       <c r="G14">
-        <f>1-F14</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H14" s="4" t="s">
@@ -6191,7 +6177,7 @@
         <v>1</v>
       </c>
       <c r="G15">
-        <f>1-F15</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H15" s="4" t="s">
@@ -6222,7 +6208,7 @@
         <v>1</v>
       </c>
       <c r="G16">
-        <f>1-F16</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H16" s="4" t="s">
@@ -6253,7 +6239,7 @@
         <v>1</v>
       </c>
       <c r="G17">
-        <f>1-F17</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H17" s="4" t="s">
@@ -6284,7 +6270,7 @@
         <v>1</v>
       </c>
       <c r="G18">
-        <f>1-F18</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H18" s="4" t="s">
@@ -6315,7 +6301,7 @@
         <v>1</v>
       </c>
       <c r="G19">
-        <f>1-F19</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H19" s="4" t="s">
@@ -6346,7 +6332,7 @@
         <v>1</v>
       </c>
       <c r="G20">
-        <f>1-F20</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H20" s="4" t="s">
@@ -6377,7 +6363,7 @@
         <v>1</v>
       </c>
       <c r="G21">
-        <f>1-F21</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H21" s="4" t="s">
@@ -6408,7 +6394,7 @@
         <v>1</v>
       </c>
       <c r="G22">
-        <f>1-F22</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H22" s="4" t="s">
@@ -6439,7 +6425,7 @@
         <v>1</v>
       </c>
       <c r="G23">
-        <f>1-F23</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H23" s="4" t="s">
@@ -6470,7 +6456,7 @@
         <v>1</v>
       </c>
       <c r="G24">
-        <f>1-F24</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H24" s="4" t="s">
@@ -6501,7 +6487,7 @@
         <v>1</v>
       </c>
       <c r="G25">
-        <f>1-F25</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H25" s="4" t="s">
@@ -6532,7 +6518,7 @@
         <v>1</v>
       </c>
       <c r="G26">
-        <f>1-F26</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H26" s="4" t="s">
@@ -6563,7 +6549,7 @@
         <v>1</v>
       </c>
       <c r="G27">
-        <f>1-F27</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H27" s="4" t="s">
@@ -6594,7 +6580,7 @@
         <v>1</v>
       </c>
       <c r="G28">
-        <f>1-F28</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H28" s="4" t="s">
@@ -6625,7 +6611,7 @@
         <v>1</v>
       </c>
       <c r="G29">
-        <f>1-F29</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H29" s="4" t="s">
@@ -6656,7 +6642,7 @@
         <v>1</v>
       </c>
       <c r="G30">
-        <f>1-F30</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H30" s="4" t="s">
@@ -6687,7 +6673,7 @@
         <v>1</v>
       </c>
       <c r="G31">
-        <f>1-F31</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H31" s="4" t="s">
@@ -6718,7 +6704,7 @@
         <v>1</v>
       </c>
       <c r="G32">
-        <f>1-F32</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H32" s="4" t="s">
@@ -6749,7 +6735,7 @@
         <v>1</v>
       </c>
       <c r="G33">
-        <f>1-F33</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H33" s="4" t="s">
@@ -6780,7 +6766,7 @@
         <v>1</v>
       </c>
       <c r="G34">
-        <f>1-F34</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H34" s="4" t="s">
@@ -6811,7 +6797,7 @@
         <v>1</v>
       </c>
       <c r="G35">
-        <f>1-F35</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H35" s="4" t="s">
@@ -6842,7 +6828,7 @@
         <v>1</v>
       </c>
       <c r="G36">
-        <f>1-F36</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H36" s="4" t="s">
@@ -6873,7 +6859,7 @@
         <v>1</v>
       </c>
       <c r="G37">
-        <f>1-F37</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H37" s="4" t="s">
@@ -6904,7 +6890,7 @@
         <v>1</v>
       </c>
       <c r="G38">
-        <f>1-F38</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H38" s="4" t="s">
@@ -6935,7 +6921,7 @@
         <v>1</v>
       </c>
       <c r="G39">
-        <f>1-F39</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H39" s="4" t="s">
@@ -6966,7 +6952,7 @@
         <v>1</v>
       </c>
       <c r="G40">
-        <f>1-F40</f>
+        <f t="shared" ref="G40:G71" si="1">1-F40</f>
         <v>0</v>
       </c>
       <c r="H40" s="4" t="s">
@@ -6997,7 +6983,7 @@
         <v>1</v>
       </c>
       <c r="G41">
-        <f>1-F41</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H41" s="4" t="s">
@@ -7028,7 +7014,7 @@
         <v>1</v>
       </c>
       <c r="G42">
-        <f>1-F42</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H42" s="4" t="s">
@@ -7059,7 +7045,7 @@
         <v>1</v>
       </c>
       <c r="G43">
-        <f>1-F43</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H43" s="4" t="s">
@@ -7090,7 +7076,7 @@
         <v>1</v>
       </c>
       <c r="G44">
-        <f>1-F44</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H44" s="4" t="s">
@@ -7121,7 +7107,7 @@
         <v>1</v>
       </c>
       <c r="G45">
-        <f>1-F45</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H45" s="4" t="s">
@@ -7152,7 +7138,7 @@
         <v>1</v>
       </c>
       <c r="G46">
-        <f>1-F46</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H46" s="4" t="s">
@@ -7183,7 +7169,7 @@
         <v>1</v>
       </c>
       <c r="G47">
-        <f>1-F47</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H47" s="4" t="s">
@@ -7214,7 +7200,7 @@
         <v>1</v>
       </c>
       <c r="G48">
-        <f>1-F48</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H48" s="4" t="s">
@@ -7245,7 +7231,7 @@
         <v>1</v>
       </c>
       <c r="G49">
-        <f>1-F49</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H49" s="4" t="s">
@@ -7276,7 +7262,7 @@
         <v>1</v>
       </c>
       <c r="G50">
-        <f>1-F50</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H50" s="4" t="s">
@@ -7307,7 +7293,7 @@
         <v>1</v>
       </c>
       <c r="G51">
-        <f>1-F51</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H51" s="4" t="s">
@@ -7338,7 +7324,7 @@
         <v>1</v>
       </c>
       <c r="G52">
-        <f>1-F52</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H52" s="4" t="s">
@@ -7369,7 +7355,7 @@
         <v>1</v>
       </c>
       <c r="G53">
-        <f>1-F53</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H53" s="4" t="s">
@@ -7400,7 +7386,7 @@
         <v>1</v>
       </c>
       <c r="G54">
-        <f>1-F54</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H54" s="4" t="s">
@@ -7431,7 +7417,7 @@
         <v>1</v>
       </c>
       <c r="G55">
-        <f>1-F55</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H55" t="s">
@@ -7462,7 +7448,7 @@
         <v>1</v>
       </c>
       <c r="G56">
-        <f>1-F56</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H56" t="s">
@@ -7487,14 +7473,14 @@
         <v>339</v>
       </c>
       <c r="E57">
-        <f>15.71/2</f>
+        <f t="shared" ref="E57:E65" si="2">15.71/2</f>
         <v>7.8550000000000004</v>
       </c>
       <c r="F57">
         <v>0</v>
       </c>
       <c r="G57">
-        <f>1-F57</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="H57" t="s">
@@ -7519,14 +7505,14 @@
         <v>339</v>
       </c>
       <c r="E58">
-        <f>15.71/2</f>
+        <f t="shared" si="2"/>
         <v>7.8550000000000004</v>
       </c>
       <c r="F58">
         <v>0</v>
       </c>
       <c r="G58">
-        <f>1-F58</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="H58" t="s">
@@ -7551,14 +7537,14 @@
         <v>339</v>
       </c>
       <c r="E59">
-        <f>15.71/2</f>
+        <f t="shared" si="2"/>
         <v>7.8550000000000004</v>
       </c>
       <c r="F59">
         <v>0</v>
       </c>
       <c r="G59">
-        <f>1-F59</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="H59" t="s">
@@ -7583,14 +7569,14 @@
         <v>339</v>
       </c>
       <c r="E60">
-        <f>15.71/2</f>
+        <f t="shared" si="2"/>
         <v>7.8550000000000004</v>
       </c>
       <c r="F60">
         <v>0</v>
       </c>
       <c r="G60">
-        <f>1-F60</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="H60" t="s">
@@ -7615,14 +7601,14 @@
         <v>339</v>
       </c>
       <c r="E61">
-        <f>15.71/2</f>
+        <f t="shared" si="2"/>
         <v>7.8550000000000004</v>
       </c>
       <c r="F61">
         <v>0</v>
       </c>
       <c r="G61">
-        <f>1-F61</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="H61" t="s">
@@ -7647,14 +7633,14 @@
         <v>339</v>
       </c>
       <c r="E62">
-        <f>15.71/2</f>
+        <f t="shared" si="2"/>
         <v>7.8550000000000004</v>
       </c>
       <c r="F62">
         <v>0</v>
       </c>
       <c r="G62">
-        <f>1-F62</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="H62" t="s">
@@ -7679,14 +7665,14 @@
         <v>339</v>
       </c>
       <c r="E63">
-        <f>15.71/2</f>
+        <f t="shared" si="2"/>
         <v>7.8550000000000004</v>
       </c>
       <c r="F63">
         <v>0</v>
       </c>
       <c r="G63">
-        <f>1-F63</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="H63" t="s">
@@ -7711,14 +7697,14 @@
         <v>339</v>
       </c>
       <c r="E64">
-        <f>15.71/2</f>
+        <f t="shared" si="2"/>
         <v>7.8550000000000004</v>
       </c>
       <c r="F64">
         <v>0</v>
       </c>
       <c r="G64">
-        <f>1-F64</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="H64" t="s">
@@ -7743,14 +7729,14 @@
         <v>339</v>
       </c>
       <c r="E65">
-        <f>15.71/2</f>
+        <f t="shared" si="2"/>
         <v>7.8550000000000004</v>
       </c>
       <c r="F65">
         <v>0</v>
       </c>
       <c r="G65">
-        <f>1-F65</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="H65" t="s">
@@ -7781,7 +7767,7 @@
         <v>1</v>
       </c>
       <c r="G66">
-        <f>1-F66</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H66" s="4" t="s">
@@ -7812,7 +7798,7 @@
         <v>1</v>
       </c>
       <c r="G67">
-        <f>1-F67</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H67" s="4" t="s">
@@ -7843,7 +7829,7 @@
         <v>1</v>
       </c>
       <c r="G68">
-        <f>1-F68</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H68" s="4" t="s">
@@ -7874,7 +7860,7 @@
         <v>1</v>
       </c>
       <c r="G69">
-        <f>1-F69</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H69" s="4" t="s">
@@ -7905,7 +7891,7 @@
         <v>1</v>
       </c>
       <c r="G70">
-        <f>1-F70</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H70" s="4" t="s">
@@ -7936,7 +7922,7 @@
         <v>1</v>
       </c>
       <c r="G71">
-        <f>1-F71</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H71" s="4" t="s">
@@ -7967,7 +7953,7 @@
         <v>1</v>
       </c>
       <c r="G72">
-        <f>1-F72</f>
+        <f t="shared" ref="G72:G103" si="3">1-F72</f>
         <v>0</v>
       </c>
       <c r="H72" s="4" t="s">
@@ -7998,7 +7984,7 @@
         <v>1</v>
       </c>
       <c r="G73">
-        <f>1-F73</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H73" s="4" t="s">
@@ -8029,7 +8015,7 @@
         <v>0</v>
       </c>
       <c r="G74">
-        <f>1-F74</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H74" t="s">
@@ -8060,7 +8046,7 @@
         <v>1</v>
       </c>
       <c r="G75">
-        <f>1-F75</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H75" s="4" t="s">
@@ -8091,7 +8077,7 @@
         <v>1</v>
       </c>
       <c r="G76">
-        <f>1-F76</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H76" s="4" t="s">
@@ -8122,7 +8108,7 @@
         <v>1</v>
       </c>
       <c r="G77">
-        <f>1-F77</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H77" s="4" t="s">
@@ -8153,7 +8139,7 @@
         <v>1</v>
       </c>
       <c r="G78">
-        <f>1-F78</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H78" s="4" t="s">
@@ -8184,7 +8170,7 @@
         <v>1</v>
       </c>
       <c r="G79">
-        <f>1-F79</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H79" s="4" t="s">
@@ -8215,7 +8201,7 @@
         <v>1</v>
       </c>
       <c r="G80">
-        <f>1-F80</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H80" s="4" t="s">
@@ -8246,7 +8232,7 @@
         <v>1</v>
       </c>
       <c r="G81">
-        <f>1-F81</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H81" s="4" t="s">
@@ -8277,7 +8263,7 @@
         <v>1</v>
       </c>
       <c r="G82">
-        <f>1-F82</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H82" s="4" t="s">
@@ -8308,7 +8294,7 @@
         <v>1</v>
       </c>
       <c r="G83">
-        <f>1-F83</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H83" s="4" t="s">
@@ -8339,7 +8325,7 @@
         <v>1</v>
       </c>
       <c r="G84">
-        <f>1-F84</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H84" s="4" t="s">
@@ -8370,7 +8356,7 @@
         <v>1</v>
       </c>
       <c r="G85">
-        <f>1-F85</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H85" s="4" t="s">
@@ -8401,7 +8387,7 @@
         <v>1</v>
       </c>
       <c r="G86">
-        <f>1-F86</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H86" s="4" t="s">
@@ -8432,7 +8418,7 @@
         <v>1</v>
       </c>
       <c r="G87">
-        <f>1-F87</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H87" s="4" t="s">
@@ -8463,7 +8449,7 @@
         <v>1</v>
       </c>
       <c r="G88">
-        <f>1-F88</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H88" t="s">
@@ -8494,7 +8480,7 @@
         <v>0</v>
       </c>
       <c r="G89">
-        <f>1-F89</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H89" s="4" t="s">
@@ -8525,7 +8511,7 @@
         <v>0</v>
       </c>
       <c r="G90">
-        <f>1-F90</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H90" s="4" t="s">
@@ -8556,7 +8542,7 @@
         <v>0</v>
       </c>
       <c r="G91">
-        <f>1-F91</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H91" s="4" t="s">
@@ -8587,7 +8573,7 @@
         <v>0</v>
       </c>
       <c r="G92">
-        <f>1-F92</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H92" s="4" t="s">
@@ -8618,7 +8604,7 @@
         <v>0</v>
       </c>
       <c r="G93">
-        <f>1-F93</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H93" s="4" t="s">
@@ -8649,7 +8635,7 @@
         <v>0</v>
       </c>
       <c r="G94">
-        <f>1-F94</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H94" s="4" t="s">
@@ -8680,7 +8666,7 @@
         <v>0</v>
       </c>
       <c r="G95">
-        <f>1-F95</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H95" s="4" t="s">
@@ -8711,7 +8697,7 @@
         <v>1</v>
       </c>
       <c r="G96">
-        <f>1-F96</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H96" s="4" t="s">
@@ -8742,7 +8728,7 @@
         <v>1</v>
       </c>
       <c r="G97">
-        <f>1-F97</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H97" t="s">
@@ -8773,7 +8759,7 @@
         <v>1</v>
       </c>
       <c r="G98">
-        <f>1-F98</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H98" t="s">
@@ -8804,7 +8790,7 @@
         <v>1</v>
       </c>
       <c r="G99">
-        <f>1-F99</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H99" s="4" t="s">
@@ -8835,7 +8821,7 @@
         <v>0</v>
       </c>
       <c r="G100">
-        <f>1-F100</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H100" s="4" t="s">
@@ -8866,7 +8852,7 @@
         <v>1</v>
       </c>
       <c r="G101">
-        <f>1-F101</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H101" s="4" t="s">
@@ -8897,7 +8883,7 @@
         <v>1</v>
       </c>
       <c r="G102">
-        <f>1-F102</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H102" t="s">
@@ -8928,7 +8914,7 @@
         <v>0</v>
       </c>
       <c r="G103">
-        <f>1-F103</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H103" s="4" t="s">
@@ -8959,7 +8945,7 @@
         <v>0</v>
       </c>
       <c r="G104">
-        <f>1-F104</f>
+        <f t="shared" ref="G104:G135" si="4">1-F104</f>
         <v>1</v>
       </c>
       <c r="H104" s="4" t="s">
@@ -8990,7 +8976,7 @@
         <v>0</v>
       </c>
       <c r="G105">
-        <f>1-F105</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="H105" s="4" t="s">
@@ -9021,7 +9007,7 @@
         <v>0</v>
       </c>
       <c r="G106">
-        <f>1-F106</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="H106" s="4" t="s">
@@ -9052,7 +9038,7 @@
         <v>0</v>
       </c>
       <c r="G107">
-        <f>1-F107</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="H107" s="4" t="s">
@@ -9083,7 +9069,7 @@
         <v>0</v>
       </c>
       <c r="G108">
-        <f>1-F108</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="H108" s="4" t="s">
@@ -9114,7 +9100,7 @@
         <v>0</v>
       </c>
       <c r="G109">
-        <f>1-F109</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="H109" s="4" t="s">
@@ -9145,7 +9131,7 @@
         <v>0</v>
       </c>
       <c r="G110">
-        <f>1-F110</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="H110" s="4" t="s">
@@ -9176,7 +9162,7 @@
         <v>0</v>
       </c>
       <c r="G111">
-        <f>1-F111</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="H111" s="4" t="s">
@@ -9207,7 +9193,7 @@
         <v>0</v>
       </c>
       <c r="G112">
-        <f>1-F112</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="H112" s="4" t="s">
@@ -9238,7 +9224,7 @@
         <v>1</v>
       </c>
       <c r="G113">
-        <f>1-F113</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H113" t="s">
@@ -9269,7 +9255,7 @@
         <v>1</v>
       </c>
       <c r="G114">
-        <f>1-F114</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H114" t="s">
@@ -9300,7 +9286,7 @@
         <v>1</v>
       </c>
       <c r="G115">
-        <f>1-F115</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H115" t="s">
@@ -9331,7 +9317,7 @@
         <v>1</v>
       </c>
       <c r="G116">
-        <f>1-F116</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H116" s="4" t="s">
@@ -9362,7 +9348,7 @@
         <v>1</v>
       </c>
       <c r="G117">
-        <f>1-F117</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H117" s="4" t="s">
@@ -9393,7 +9379,7 @@
         <v>1</v>
       </c>
       <c r="G118">
-        <f>1-F118</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H118" s="4" t="s">
@@ -9424,7 +9410,7 @@
         <v>1</v>
       </c>
       <c r="G119">
-        <f>1-F119</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H119" s="4" t="s">
@@ -9455,7 +9441,7 @@
         <v>1</v>
       </c>
       <c r="G120">
-        <f>1-F120</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H120" s="4" t="s">
@@ -9486,7 +9472,7 @@
         <v>1</v>
       </c>
       <c r="G121">
-        <f>1-F121</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H121" s="4" t="s">
@@ -9517,7 +9503,7 @@
         <v>1</v>
       </c>
       <c r="G122">
-        <f>1-F122</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H122" s="4" t="s">
@@ -9548,7 +9534,7 @@
         <v>1</v>
       </c>
       <c r="G123">
-        <f>1-F123</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H123" s="4" t="s">
@@ -9579,7 +9565,7 @@
         <v>1</v>
       </c>
       <c r="G124">
-        <f>1-F124</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H124" s="4" t="s">
@@ -9610,7 +9596,7 @@
         <v>1</v>
       </c>
       <c r="G125">
-        <f>1-F125</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H125" s="4" t="s">
@@ -9641,7 +9627,7 @@
         <v>1</v>
       </c>
       <c r="G126">
-        <f>1-F126</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H126" s="4" t="s">
@@ -9672,7 +9658,7 @@
         <v>1</v>
       </c>
       <c r="G127">
-        <f>1-F127</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H127" s="4" t="s">
@@ -9703,7 +9689,7 @@
         <v>1</v>
       </c>
       <c r="G128">
-        <f>1-F128</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H128" s="4" t="s">
@@ -9734,7 +9720,7 @@
         <v>1</v>
       </c>
       <c r="G129">
-        <f>1-F129</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H129" s="4" t="s">
@@ -9765,7 +9751,7 @@
         <v>1</v>
       </c>
       <c r="G130">
-        <f>1-F130</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H130" s="4" t="s">
@@ -9796,7 +9782,7 @@
         <v>1</v>
       </c>
       <c r="G131">
-        <f>1-F131</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H131" s="4" t="s">
@@ -9827,7 +9813,7 @@
         <v>1</v>
       </c>
       <c r="G132">
-        <f>1-F132</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H132" s="4" t="s">
@@ -9858,7 +9844,7 @@
         <v>1</v>
       </c>
       <c r="G133">
-        <f>1-F133</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H133" s="4" t="s">
@@ -9889,7 +9875,7 @@
         <v>1</v>
       </c>
       <c r="G134">
-        <f>1-F134</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H134" s="4" t="s">
@@ -9920,7 +9906,7 @@
         <v>1</v>
       </c>
       <c r="G135">
-        <f>1-F135</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H135" s="4" t="s">
@@ -9951,7 +9937,7 @@
         <v>1</v>
       </c>
       <c r="G136">
-        <f>1-F136</f>
+        <f t="shared" ref="G136:G167" si="5">1-F136</f>
         <v>0</v>
       </c>
       <c r="H136" s="4" t="s">
@@ -9982,7 +9968,7 @@
         <v>1</v>
       </c>
       <c r="G137">
-        <f>1-F137</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="H137" s="4" t="s">
@@ -10013,7 +9999,7 @@
         <v>1</v>
       </c>
       <c r="G138">
-        <f>1-F138</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="H138" s="4" t="s">
@@ -10044,7 +10030,7 @@
         <v>1</v>
       </c>
       <c r="G139">
-        <f>1-F139</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="H139" s="4" t="s">
@@ -10075,7 +10061,7 @@
         <v>1</v>
       </c>
       <c r="G140">
-        <f>1-F140</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="H140" s="4" t="s">
@@ -10106,7 +10092,7 @@
         <v>1</v>
       </c>
       <c r="G141">
-        <f>1-F141</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="H141" s="4" t="s">
@@ -10171,7 +10157,7 @@
         <v>0</v>
       </c>
       <c r="H143" t="s">
-        <v>212</v>
+        <v>352</v>
       </c>
       <c r="J143" s="3" t="s">
         <v>263</v>

</xml_diff>